<commit_message>
update zone maps to include epsdp
</commit_message>
<xml_diff>
--- a/mock_tables/zone_maps.xlsx
+++ b/mock_tables/zone_maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtse\source\Workspaces\QuoteTestApp\mock_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E7F9ED-9036-44C5-A589-59BA2DD6A6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A011F1E0-02DD-4127-B320-22D7BD5B456B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4817" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4818" uniqueCount="720">
   <si>
     <t>ORIGINAL_SERVICE</t>
   </si>
@@ -2589,11 +2589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2437"/>
+  <dimension ref="A1:G2438"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E220" sqref="E220"/>
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D234" sqref="D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58150,11 +58150,33 @@
         <v>8</v>
       </c>
       <c r="F2437" t="str">
-        <f t="shared" ref="F2437" si="78">VLOOKUP(B2437,cty_names,3,FALSE)</f>
+        <f t="shared" ref="F2437:F2438" si="78">VLOOKUP(B2437,cty_names,3,FALSE)</f>
         <v>Zimbabwe</v>
       </c>
       <c r="G2437">
         <v>44</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2438">
+        <v>98</v>
+      </c>
+      <c r="B2438" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2438">
+        <v>1</v>
+      </c>
+      <c r="D2438" t="str">
+        <f t="shared" ref="D2438" si="79">VLOOKUP(C2438,eps_zones,2,FALSE)</f>
+        <v xml:space="preserve"> Canada  </v>
+      </c>
+      <c r="E2438">
+        <v>1</v>
+      </c>
+      <c r="F2438" t="str">
+        <f t="shared" si="78"/>
+        <v>Canada</v>
       </c>
     </row>
   </sheetData>

</xml_diff>